<commit_message>
fixed segregation function in interdependence script. now origin and outside have segregation by region
</commit_message>
<xml_diff>
--- a/src/R/helpers/population.xlsx
+++ b/src/R/helpers/population.xlsx
@@ -9,25 +9,26 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6780" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6780" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="population" sheetId="1" r:id="rId1"/>
     <sheet name="region_countries" sheetId="2" r:id="rId2"/>
     <sheet name="population_region_country" sheetId="3" r:id="rId3"/>
+    <sheet name="population_region" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">population!$A$1:$E$275</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="307">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -1431,10 +1432,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3825,7 +3827,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A1:F253" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
@@ -4973,6 +4975,423 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A1:E25" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="232">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="95"/>
+        <item x="96"/>
+        <item x="97"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="100"/>
+        <item x="101"/>
+        <item x="102"/>
+        <item x="103"/>
+        <item x="104"/>
+        <item x="105"/>
+        <item x="106"/>
+        <item x="107"/>
+        <item x="108"/>
+        <item x="109"/>
+        <item x="110"/>
+        <item x="111"/>
+        <item x="112"/>
+        <item x="113"/>
+        <item x="114"/>
+        <item x="115"/>
+        <item x="116"/>
+        <item x="117"/>
+        <item x="118"/>
+        <item x="119"/>
+        <item x="120"/>
+        <item x="121"/>
+        <item x="122"/>
+        <item x="123"/>
+        <item x="124"/>
+        <item x="125"/>
+        <item x="126"/>
+        <item x="127"/>
+        <item x="128"/>
+        <item x="129"/>
+        <item x="130"/>
+        <item x="131"/>
+        <item x="132"/>
+        <item x="133"/>
+        <item x="134"/>
+        <item x="135"/>
+        <item x="136"/>
+        <item x="137"/>
+        <item x="138"/>
+        <item x="139"/>
+        <item x="140"/>
+        <item x="141"/>
+        <item x="142"/>
+        <item x="143"/>
+        <item x="144"/>
+        <item x="145"/>
+        <item x="146"/>
+        <item x="147"/>
+        <item x="148"/>
+        <item x="149"/>
+        <item x="150"/>
+        <item x="151"/>
+        <item x="152"/>
+        <item x="153"/>
+        <item x="154"/>
+        <item x="155"/>
+        <item x="156"/>
+        <item x="157"/>
+        <item x="158"/>
+        <item x="159"/>
+        <item x="160"/>
+        <item x="161"/>
+        <item x="162"/>
+        <item x="163"/>
+        <item x="164"/>
+        <item x="165"/>
+        <item x="166"/>
+        <item x="167"/>
+        <item x="168"/>
+        <item x="169"/>
+        <item x="170"/>
+        <item x="171"/>
+        <item x="172"/>
+        <item x="173"/>
+        <item x="174"/>
+        <item x="175"/>
+        <item x="176"/>
+        <item x="177"/>
+        <item x="178"/>
+        <item x="179"/>
+        <item x="180"/>
+        <item x="181"/>
+        <item x="182"/>
+        <item x="183"/>
+        <item x="184"/>
+        <item x="185"/>
+        <item x="186"/>
+        <item x="187"/>
+        <item x="188"/>
+        <item x="189"/>
+        <item x="190"/>
+        <item x="191"/>
+        <item x="192"/>
+        <item x="193"/>
+        <item x="194"/>
+        <item x="195"/>
+        <item x="196"/>
+        <item x="197"/>
+        <item x="198"/>
+        <item x="199"/>
+        <item x="200"/>
+        <item x="201"/>
+        <item x="202"/>
+        <item x="203"/>
+        <item x="204"/>
+        <item x="205"/>
+        <item x="206"/>
+        <item x="207"/>
+        <item x="208"/>
+        <item x="209"/>
+        <item x="210"/>
+        <item x="211"/>
+        <item x="212"/>
+        <item x="213"/>
+        <item x="214"/>
+        <item x="215"/>
+        <item x="216"/>
+        <item x="217"/>
+        <item x="218"/>
+        <item x="219"/>
+        <item x="220"/>
+        <item x="221"/>
+        <item x="222"/>
+        <item x="223"/>
+        <item x="224"/>
+        <item x="225"/>
+        <item x="226"/>
+        <item x="227"/>
+        <item x="228"/>
+        <item x="229"/>
+        <item x="230"/>
+        <item t="default"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="25">
+        <item x="4"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="18"/>
+        <item x="20"/>
+        <item x="12"/>
+        <item x="1"/>
+        <item x="21"/>
+        <item x="19"/>
+        <item x="9"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="15"/>
+        <item x="7"/>
+        <item x="16"/>
+        <item x="11"/>
+        <item x="17"/>
+        <item x="2"/>
+        <item x="14"/>
+        <item x="0"/>
+        <item x="10"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item t="default"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="24">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+  </colItems>
+  <dataFields count="4">
+    <dataField name="Sum of 2010" fld="2" baseField="0" baseItem="4"/>
+    <dataField name="Sum of 2011" fld="3" baseField="0" baseItem="4"/>
+    <dataField name="Sum of 2012" fld="4" baseField="0" baseItem="4"/>
+    <dataField name="Sum of 2013" fld="5" baseField="0" baseItem="4"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5238,8 +5657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E275"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="E226" sqref="E226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9821,8 +10240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F251"/>
   <sheetViews>
-    <sheetView topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="B251" sqref="B251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15864,8 +16283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F251" sqref="A2:F251"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20990,4 +21409,504 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="6" width="12" customWidth="1"/>
+    <col min="7" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="32" width="8" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7" bestFit="1" customWidth="1"/>
+    <col min="34" max="39" width="8" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7" bestFit="1" customWidth="1"/>
+    <col min="41" max="46" width="8" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="7" bestFit="1" customWidth="1"/>
+    <col min="49" max="53" width="8" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="7" bestFit="1" customWidth="1"/>
+    <col min="55" max="61" width="8" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="7" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8" bestFit="1" customWidth="1"/>
+    <col min="64" max="68" width="9" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="7" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="9" bestFit="1" customWidth="1"/>
+    <col min="71" max="72" width="8" bestFit="1" customWidth="1"/>
+    <col min="73" max="79" width="9" bestFit="1" customWidth="1"/>
+    <col min="80" max="82" width="8" bestFit="1" customWidth="1"/>
+    <col min="83" max="85" width="9" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="8" bestFit="1" customWidth="1"/>
+    <col min="87" max="100" width="9" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="8" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="9" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="8" bestFit="1" customWidth="1"/>
+    <col min="104" max="106" width="9" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="8" bestFit="1" customWidth="1"/>
+    <col min="108" max="113" width="9" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="8" bestFit="1" customWidth="1"/>
+    <col min="115" max="116" width="9" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="8" bestFit="1" customWidth="1"/>
+    <col min="118" max="120" width="9" bestFit="1" customWidth="1"/>
+    <col min="121" max="122" width="8" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="9" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="8" bestFit="1" customWidth="1"/>
+    <col min="125" max="128" width="9" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="8" bestFit="1" customWidth="1"/>
+    <col min="130" max="136" width="9" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="8" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="9" bestFit="1" customWidth="1"/>
+    <col min="139" max="142" width="10" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="9" bestFit="1" customWidth="1"/>
+    <col min="144" max="151" width="10" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="9" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="10" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="9" bestFit="1" customWidth="1"/>
+    <col min="155" max="166" width="10" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="9" bestFit="1" customWidth="1"/>
+    <col min="168" max="193" width="10" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="9" bestFit="1" customWidth="1"/>
+    <col min="195" max="198" width="10" bestFit="1" customWidth="1"/>
+    <col min="199" max="199" width="9" bestFit="1" customWidth="1"/>
+    <col min="200" max="206" width="10" bestFit="1" customWidth="1"/>
+    <col min="207" max="207" width="9" bestFit="1" customWidth="1"/>
+    <col min="208" max="209" width="10" bestFit="1" customWidth="1"/>
+    <col min="210" max="218" width="11" bestFit="1" customWidth="1"/>
+    <col min="219" max="221" width="12" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="7" bestFit="1" customWidth="1"/>
+    <col min="224" max="224" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B2" s="3">
+        <v>119464.19700000001</v>
+      </c>
+      <c r="C2" s="3">
+        <v>123311.68299999999</v>
+      </c>
+      <c r="D2" s="3">
+        <v>127259.29299999999</v>
+      </c>
+      <c r="E2" s="3">
+        <v>131309.196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B3" s="3">
+        <v>160556.595</v>
+      </c>
+      <c r="C3" s="3">
+        <v>163028.36400000003</v>
+      </c>
+      <c r="D3" s="3">
+        <v>165467.12400000001</v>
+      </c>
+      <c r="E3" s="3">
+        <v>167875.53599999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" s="3">
+        <v>41743.924000000006</v>
+      </c>
+      <c r="C4" s="3">
+        <v>41858.532000000007</v>
+      </c>
+      <c r="D4" s="3">
+        <v>42176.284000000007</v>
+      </c>
+      <c r="E4" s="3">
+        <v>42492.200000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B5" s="3">
+        <v>222451.745</v>
+      </c>
+      <c r="C5" s="3">
+        <v>223669.41899999999</v>
+      </c>
+      <c r="D5" s="3">
+        <v>224994.16200000001</v>
+      </c>
+      <c r="E5" s="3">
+        <v>226376.82700000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B6" s="3">
+        <v>243730.09100000001</v>
+      </c>
+      <c r="C6" s="3">
+        <v>250548.34499999997</v>
+      </c>
+      <c r="D6" s="3">
+        <v>257520.55900000004</v>
+      </c>
+      <c r="E6" s="3">
+        <v>264641.07900000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2986248.3730000001</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3002294.9279999998</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3018309.78</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3034052.2089999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>287</v>
+      </c>
+      <c r="B8" s="3">
+        <v>283174.55800000002</v>
+      </c>
+      <c r="C8" s="3">
+        <v>282808.951</v>
+      </c>
+      <c r="D8" s="3">
+        <v>282519.33</v>
+      </c>
+      <c r="E8" s="3">
+        <v>282268.03800000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>276</v>
+      </c>
+      <c r="B9" s="3">
+        <v>123047.15100000001</v>
+      </c>
+      <c r="C9" s="3">
+        <v>123909.236</v>
+      </c>
+      <c r="D9" s="3">
+        <v>124830.709</v>
+      </c>
+      <c r="E9" s="3">
+        <v>125805.14299999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>296</v>
+      </c>
+      <c r="B10" s="3">
+        <v>24011.210999999996</v>
+      </c>
+      <c r="C10" s="3">
+        <v>24630.679</v>
+      </c>
+      <c r="D10" s="3">
+        <v>25260.003999999997</v>
+      </c>
+      <c r="E10" s="3">
+        <v>25901.101000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>294</v>
+      </c>
+      <c r="B11" s="3">
+        <v>342872.97100000002</v>
+      </c>
+      <c r="C11" s="3">
+        <v>345652.821</v>
+      </c>
+      <c r="D11" s="3">
+        <v>348298.87400000001</v>
+      </c>
+      <c r="E11" s="3">
+        <v>350854.85800000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>284</v>
+      </c>
+      <c r="B12" s="3">
+        <v>26490.125999999997</v>
+      </c>
+      <c r="C12" s="3">
+        <v>26898.163999999997</v>
+      </c>
+      <c r="D12" s="3">
+        <v>27289.591999999997</v>
+      </c>
+      <c r="E12" s="3">
+        <v>27668.256000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>278</v>
+      </c>
+      <c r="B13" s="3">
+        <v>10070.546</v>
+      </c>
+      <c r="C13" s="3">
+        <v>10265.328</v>
+      </c>
+      <c r="D13" s="3">
+        <v>10460.377999999999</v>
+      </c>
+      <c r="E13" s="3">
+        <v>10656.185999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>280</v>
+      </c>
+      <c r="B14" s="3">
+        <v>195812.842</v>
+      </c>
+      <c r="C14" s="3">
+        <v>200831.54699999999</v>
+      </c>
+      <c r="D14" s="3">
+        <v>206057.486</v>
+      </c>
+      <c r="E14" s="3">
+        <v>211459.49100000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>290</v>
+      </c>
+      <c r="B15" s="3">
+        <v>117138.02900000001</v>
+      </c>
+      <c r="C15" s="3">
+        <v>118575.69</v>
+      </c>
+      <c r="D15" s="3">
+        <v>120008.857</v>
+      </c>
+      <c r="E15" s="3">
+        <v>121433.49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>282</v>
+      </c>
+      <c r="B16" s="3">
+        <v>61594.51</v>
+      </c>
+      <c r="C16" s="3">
+        <v>62198.716</v>
+      </c>
+      <c r="D16" s="3">
+        <v>62806.12</v>
+      </c>
+      <c r="E16" s="3">
+        <v>63413.782000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17" s="3">
+        <v>333685.69399999996</v>
+      </c>
+      <c r="C17" s="3">
+        <v>337387.43799999997</v>
+      </c>
+      <c r="D17" s="3">
+        <v>341070.02400000003</v>
+      </c>
+      <c r="E17" s="3">
+        <v>344717.85200000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>286</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1431443.4350000001</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1449905.7500000002</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1468006.5549999999</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1485808.4000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>292</v>
+      </c>
+      <c r="B19" s="3">
+        <v>604436.01</v>
+      </c>
+      <c r="C19" s="3">
+        <v>611982.65800000005</v>
+      </c>
+      <c r="D19" s="3">
+        <v>619653.04099999997</v>
+      </c>
+      <c r="E19" s="3">
+        <v>627370.03799999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>277</v>
+      </c>
+      <c r="B20" s="3">
+        <v>287330.73700000002</v>
+      </c>
+      <c r="C20" s="3">
+        <v>292258.51999999996</v>
+      </c>
+      <c r="D20" s="3">
+        <v>297247.28000000003</v>
+      </c>
+      <c r="E20" s="3">
+        <v>302270.22300000006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>289</v>
+      </c>
+      <c r="B21" s="3">
+        <v>320144.46299999993</v>
+      </c>
+      <c r="C21" s="3">
+        <v>329084.29099999997</v>
+      </c>
+      <c r="D21" s="3">
+        <v>338265.13500000001</v>
+      </c>
+      <c r="E21" s="3">
+        <v>347677.022</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>275</v>
+      </c>
+      <c r="B22" s="3">
+        <v>489414.84799999994</v>
+      </c>
+      <c r="C22" s="3">
+        <v>500117.25000000006</v>
+      </c>
+      <c r="D22" s="3">
+        <v>510899.01000000007</v>
+      </c>
+      <c r="E22" s="3">
+        <v>521687.41200000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>285</v>
+      </c>
+      <c r="B23" s="3">
+        <v>292364.59999999998</v>
+      </c>
+      <c r="C23" s="3">
+        <v>293774.93599999999</v>
+      </c>
+      <c r="D23" s="3">
+        <v>295162.84400000004</v>
+      </c>
+      <c r="E23" s="3">
+        <v>296528.39299999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>298</v>
+      </c>
+      <c r="B24" s="3">
+        <v>180197.49799999999</v>
+      </c>
+      <c r="C24" s="3">
+        <v>180637.97399999999</v>
+      </c>
+      <c r="D24" s="3">
+        <v>180812.932</v>
+      </c>
+      <c r="E24" s="3">
+        <v>180813.14400000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>300</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>